<commit_message>
Modifications to Case Header Report for new column "Resolution Code" and changes to Duration Text.
</commit_message>
<xml_diff>
--- a/ReportLayouts/CaseHeader.xlsx
+++ b/ReportLayouts/CaseHeader.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexv\Documents\AL\Orbus2Reports\ReportLayouts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6a9ae9b926c6b4ec/AL/SMB_ERP SOL/Github/OrbusWebMaster/OrbusReports/ReportLayouts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB7897D-5334-479F-8D8F-E017513D5E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{7EB7897D-5334-479F-8D8F-E017513D5E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2B62E0B-1FC7-49ED-ACC5-1BDF2D4D91FF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>No</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>Responsible_Owner</t>
+  </si>
+  <si>
+    <t>Resolution_Code</t>
   </si>
 </sst>
 </file>
@@ -150,10 +153,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
-    <dxf>
-      <font>
-        <strike val="0"/>
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -400,23 +421,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" name="Data" displayName="Data" ref="A1:N2" insertRow="1" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="A1:N2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
-  <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="No" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="EntityName" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SalesHeaderNo" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ReasonCode" dataDxfId="10"/>
-    <tableColumn id="14" xr3:uid="{9283ADAA-49CC-422F-8808-5AF1694FC556}" name="DepartmentSpecification" dataDxfId="9"/>
-    <tableColumn id="5" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="AssignedDate" dataDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ResolutionDate" dataDxfId="7"/>
-    <tableColumn id="7" xr3:uid="{E08C6680-74C7-4CF8-9919-976A73CE18EE}" name="DurationText" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{E5B8BD56-7B2E-43FB-B15D-068682BBA541}" name="AssignedUserID" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{F225765D-CC55-4A92-B57C-6D82171AF752}" name="ReasonNotes" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{B0205E85-C19E-409B-86FD-4087297B38AF}" name="SecondCase" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{C9C7086A-1B97-489C-B958-081BCCEDA2B8}" name="Location_Code" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{C466F251-EA5C-4FC2-AD09-08287CF70C47}" name="Status" dataDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{2AB36868-025F-475A-85F3-118C122B46EA}" name="Responsible_Owner" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" name="Data" displayName="Data" ref="A1:O2" insertRow="1" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="A1:O2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="No" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="EntityName" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SalesHeaderNo" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ReasonCode" dataDxfId="11"/>
+    <tableColumn id="14" xr3:uid="{9283ADAA-49CC-422F-8808-5AF1694FC556}" name="DepartmentSpecification" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="AssignedDate" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ResolutionDate" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{E08C6680-74C7-4CF8-9919-976A73CE18EE}" name="DurationText" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{E5B8BD56-7B2E-43FB-B15D-068682BBA541}" name="AssignedUserID" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{F225765D-CC55-4A92-B57C-6D82171AF752}" name="ReasonNotes" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{B0205E85-C19E-409B-86FD-4087297B38AF}" name="SecondCase" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{C9C7086A-1B97-489C-B958-081BCCEDA2B8}" name="Location_Code" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{C466F251-EA5C-4FC2-AD09-08287CF70C47}" name="Status" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{BCD24949-DFC6-425A-AEA3-DF0B5FB1AF1E}" name="Responsible_Owner" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{741AA29D-1ED4-4DE0-9230-FEE648BDB92E}" name="Resolution_Code" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -719,32 +741,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N22" sqref="N22"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="2" max="2" width="23.88671875" customWidth="1"/>
+    <col min="3" max="3" width="18.33203125" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
     <col min="5" max="5" width="27" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1"/>
-    <col min="8" max="8" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="17.6640625" customWidth="1"/>
+    <col min="7" max="7" width="16.44140625" customWidth="1"/>
+    <col min="8" max="8" width="15.88671875" customWidth="1"/>
     <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="44.85546875" customWidth="1"/>
-    <col min="11" max="11" width="11.85546875" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" customWidth="1"/>
-    <col min="14" max="14" width="18.28515625" customWidth="1"/>
+    <col min="10" max="10" width="44.88671875" customWidth="1"/>
+    <col min="11" max="11" width="11.88671875" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" customWidth="1"/>
+    <col min="13" max="14" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -787,8 +808,11 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" s="2" customFormat="1" ht="12.75" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:15" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changes in Excel layout of case header report
</commit_message>
<xml_diff>
--- a/ReportLayouts/CaseHeader.xlsx
+++ b/ReportLayouts/CaseHeader.xlsx
@@ -1,39 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6a9ae9b926c6b4ec/AL/SMB_ERP SOL/Github/OrbusWebMaster/OrbusReports/ReportLayouts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{7EB7897D-5334-479F-8D8F-E017513D5E81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2B62E0B-1FC7-49ED-ACC5-1BDF2D4D91FF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{826046BA-C3FE-467D-B04B-05A55AFB3629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>No</t>
   </si>
@@ -78,13 +65,16 @@
   </si>
   <si>
     <t>Resolution_Code</t>
+  </si>
+  <si>
+    <t>Shipment_Date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -109,6 +99,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF4EC9B0"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -143,17 +139,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -421,33 +438,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" name="Data" displayName="Data" ref="A1:O2" insertRow="1" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
-  <autoFilter ref="A1:O2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
-  <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="No" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="EntityName" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SalesHeaderNo" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ReasonCode" dataDxfId="11"/>
-    <tableColumn id="14" xr3:uid="{9283ADAA-49CC-422F-8808-5AF1694FC556}" name="DepartmentSpecification" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="AssignedDate" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ResolutionDate" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{E08C6680-74C7-4CF8-9919-976A73CE18EE}" name="DurationText" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{E5B8BD56-7B2E-43FB-B15D-068682BBA541}" name="AssignedUserID" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{F225765D-CC55-4A92-B57C-6D82171AF752}" name="ReasonNotes" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{B0205E85-C19E-409B-86FD-4087297B38AF}" name="SecondCase" dataDxfId="4"/>
-    <tableColumn id="12" xr3:uid="{C9C7086A-1B97-489C-B958-081BCCEDA2B8}" name="Location_Code" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{C466F251-EA5C-4FC2-AD09-08287CF70C47}" name="Status" dataDxfId="2"/>
-    <tableColumn id="16" xr3:uid="{BCD24949-DFC6-425A-AEA3-DF0B5FB1AF1E}" name="Responsible_Owner" dataDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{741AA29D-1ED4-4DE0-9230-FEE648BDB92E}" name="Resolution_Code" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}" name="Data" displayName="Data" ref="A1:P2" insertRow="1" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <autoFilter ref="A1:P2" xr:uid="{41D726F2-778D-4B1C-A5EA-875FED73D050}"/>
+  <tableColumns count="16">
+    <tableColumn id="1" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="No" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="EntityName" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="SalesHeaderNo" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ReasonCode" dataDxfId="12"/>
+    <tableColumn id="14" xr3:uid="{9283ADAA-49CC-422F-8808-5AF1694FC556}" name="DepartmentSpecification" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="AssignedDate" dataDxfId="10"/>
+    <tableColumn id="15" xr3:uid="{A76C7E3D-6D57-4520-A50C-994B4B4CAB5B}" name="Shipment_Date" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ResolutionDate" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{E08C6680-74C7-4CF8-9919-976A73CE18EE}" name="DurationText" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{E5B8BD56-7B2E-43FB-B15D-068682BBA541}" name="AssignedUserID" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{F225765D-CC55-4A92-B57C-6D82171AF752}" name="ReasonNotes" dataDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{B0205E85-C19E-409B-86FD-4087297B38AF}" name="SecondCase" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{C9C7086A-1B97-489C-B958-081BCCEDA2B8}" name="Location_Code" dataDxfId="4"/>
+    <tableColumn id="11" xr3:uid="{C466F251-EA5C-4FC2-AD09-08287CF70C47}" name="Status" dataDxfId="3"/>
+    <tableColumn id="16" xr3:uid="{BCD24949-DFC6-425A-AEA3-DF0B5FB1AF1E}" name="Responsible_Owner" dataDxfId="2"/>
+    <tableColumn id="13" xr3:uid="{741AA29D-1ED4-4DE0-9230-FEE648BDB92E}" name="Resolution_Code" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -485,7 +503,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -591,7 +609,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -733,7 +751,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -741,11 +759,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -755,17 +773,17 @@
     <col min="3" max="3" width="18.33203125" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
     <col min="5" max="5" width="27" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" customWidth="1"/>
-    <col min="7" max="7" width="16.44140625" customWidth="1"/>
-    <col min="8" max="8" width="15.88671875" customWidth="1"/>
-    <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="44.88671875" customWidth="1"/>
-    <col min="11" max="11" width="11.88671875" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" customWidth="1"/>
-    <col min="13" max="14" width="14.88671875" customWidth="1"/>
+    <col min="6" max="7" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" customWidth="1"/>
+    <col min="9" max="9" width="15.88671875" customWidth="1"/>
+    <col min="10" max="10" width="20" customWidth="1"/>
+    <col min="11" max="11" width="44.88671875" customWidth="1"/>
+    <col min="12" max="12" width="11.88671875" customWidth="1"/>
+    <col min="13" max="13" width="15.33203125" customWidth="1"/>
+    <col min="14" max="15" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="4" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -784,35 +802,38 @@
       <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:16" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.3"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Formatting changed for excel layout and format has been added for shipment date
</commit_message>
<xml_diff>
--- a/ReportLayouts/CaseHeader.xlsx
+++ b/ReportLayouts/CaseHeader.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{826046BA-C3FE-467D-B04B-05A55AFB3629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F913D7C4-3783-4FE2-8298-7AC1CF034264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -99,12 +99,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF4EC9B0"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="4">
@@ -139,15 +133,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -155,6 +146,20 @@
   <dxfs count="18">
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -187,109 +192,95 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -447,16 +438,16 @@
     <tableColumn id="4" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ReasonCode" dataDxfId="12"/>
     <tableColumn id="14" xr3:uid="{9283ADAA-49CC-422F-8808-5AF1694FC556}" name="DepartmentSpecification" dataDxfId="11"/>
     <tableColumn id="5" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="AssignedDate" dataDxfId="10"/>
-    <tableColumn id="15" xr3:uid="{A76C7E3D-6D57-4520-A50C-994B4B4CAB5B}" name="Shipment_Date" dataDxfId="0"/>
-    <tableColumn id="6" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ResolutionDate" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{E08C6680-74C7-4CF8-9919-976A73CE18EE}" name="DurationText" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{E5B8BD56-7B2E-43FB-B15D-068682BBA541}" name="AssignedUserID" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{F225765D-CC55-4A92-B57C-6D82171AF752}" name="ReasonNotes" dataDxfId="6"/>
-    <tableColumn id="10" xr3:uid="{B0205E85-C19E-409B-86FD-4087297B38AF}" name="SecondCase" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{C9C7086A-1B97-489C-B958-081BCCEDA2B8}" name="Location_Code" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{C466F251-EA5C-4FC2-AD09-08287CF70C47}" name="Status" dataDxfId="3"/>
-    <tableColumn id="16" xr3:uid="{BCD24949-DFC6-425A-AEA3-DF0B5FB1AF1E}" name="Responsible_Owner" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{741AA29D-1ED4-4DE0-9230-FEE648BDB92E}" name="Resolution_Code" dataDxfId="1"/>
+    <tableColumn id="15" xr3:uid="{A76C7E3D-6D57-4520-A50C-994B4B4CAB5B}" name="Shipment_Date" dataDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{21867904-D69E-41E3-B5BE-D9B124B8D7E4}" name="ResolutionDate" dataDxfId="8"/>
+    <tableColumn id="7" xr3:uid="{E08C6680-74C7-4CF8-9919-976A73CE18EE}" name="DurationText" dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{E5B8BD56-7B2E-43FB-B15D-068682BBA541}" name="AssignedUserID" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{F225765D-CC55-4A92-B57C-6D82171AF752}" name="ReasonNotes" dataDxfId="5"/>
+    <tableColumn id="10" xr3:uid="{B0205E85-C19E-409B-86FD-4087297B38AF}" name="SecondCase" dataDxfId="4"/>
+    <tableColumn id="12" xr3:uid="{C9C7086A-1B97-489C-B958-081BCCEDA2B8}" name="Location_Code" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{C466F251-EA5C-4FC2-AD09-08287CF70C47}" name="Status" dataDxfId="2"/>
+    <tableColumn id="16" xr3:uid="{BCD24949-DFC6-425A-AEA3-DF0B5FB1AF1E}" name="Responsible_Owner" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{741AA29D-1ED4-4DE0-9230-FEE648BDB92E}" name="Resolution_Code" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -802,7 +793,7 @@
       <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H1" s="3" t="s">

</xml_diff>